<commit_message>
update norms analysis report
</commit_message>
<xml_diff>
--- a/spreadsheets/norms_analysis_31d.xlsx
+++ b/spreadsheets/norms_analysis_31d.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="3150" windowWidth="19440" windowHeight="14325"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Аркуш1!$7:$7</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -229,7 +229,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -244,7 +244,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Стандартна">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -282,7 +282,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартна">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -354,7 +354,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартна">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -940,7 +940,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -1012,1462 +1012,1462 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO9" s="7"/>
       <c r="AP9" s="7"/>
       <c r="AQ9" s="7"/>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO10" s="7"/>
       <c r="AP10" s="7"/>
       <c r="AQ10" s="7"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO11" s="7"/>
       <c r="AP11" s="7"/>
       <c r="AQ11" s="7"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO12" s="7"/>
       <c r="AP12" s="7"/>
       <c r="AQ12" s="7"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO13" s="7"/>
       <c r="AP13" s="7"/>
       <c r="AQ13" s="7"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO14" s="7"/>
       <c r="AP14" s="7"/>
       <c r="AQ14" s="7"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO15" s="7"/>
       <c r="AP15" s="7"/>
       <c r="AQ15" s="7"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO16" s="7"/>
       <c r="AP16" s="7"/>
       <c r="AQ16" s="7"/>
     </row>
-    <row r="17" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="17" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO17" s="7"/>
       <c r="AP17" s="7"/>
       <c r="AQ17" s="7"/>
     </row>
-    <row r="18" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="18" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO18" s="7"/>
       <c r="AP18" s="7"/>
       <c r="AQ18" s="7"/>
     </row>
-    <row r="19" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="19" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO19" s="7"/>
       <c r="AP19" s="7"/>
       <c r="AQ19" s="7"/>
     </row>
-    <row r="20" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="20" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO20" s="7"/>
       <c r="AP20" s="7"/>
       <c r="AQ20" s="7"/>
     </row>
-    <row r="21" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="21" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO21" s="7"/>
       <c r="AP21" s="7"/>
       <c r="AQ21" s="7"/>
     </row>
-    <row r="22" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="22" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO22" s="7"/>
       <c r="AP22" s="7"/>
       <c r="AQ22" s="7"/>
     </row>
-    <row r="23" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="23" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO23" s="7"/>
       <c r="AP23" s="7"/>
       <c r="AQ23" s="7"/>
     </row>
-    <row r="24" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="24" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO24" s="7"/>
       <c r="AP24" s="7"/>
       <c r="AQ24" s="7"/>
     </row>
-    <row r="25" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="25" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO25" s="7"/>
       <c r="AP25" s="7"/>
       <c r="AQ25" s="7"/>
     </row>
-    <row r="26" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="26" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO26" s="7"/>
       <c r="AP26" s="7"/>
       <c r="AQ26" s="7"/>
     </row>
-    <row r="27" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="27" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO27" s="7"/>
       <c r="AP27" s="7"/>
       <c r="AQ27" s="7"/>
     </row>
-    <row r="28" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="28" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO28" s="7"/>
       <c r="AP28" s="7"/>
       <c r="AQ28" s="7"/>
     </row>
-    <row r="29" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="29" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO29" s="7"/>
       <c r="AP29" s="7"/>
       <c r="AQ29" s="7"/>
     </row>
-    <row r="30" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="30" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO30" s="7"/>
       <c r="AP30" s="7"/>
       <c r="AQ30" s="7"/>
     </row>
-    <row r="31" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="31" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO31" s="7"/>
       <c r="AP31" s="7"/>
       <c r="AQ31" s="7"/>
     </row>
-    <row r="32" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="32" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO32" s="7"/>
       <c r="AP32" s="7"/>
       <c r="AQ32" s="7"/>
     </row>
-    <row r="33" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="33" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO33" s="7"/>
       <c r="AP33" s="7"/>
       <c r="AQ33" s="7"/>
     </row>
-    <row r="34" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="34" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO34" s="7"/>
       <c r="AP34" s="7"/>
       <c r="AQ34" s="7"/>
     </row>
-    <row r="35" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="35" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO35" s="7"/>
       <c r="AP35" s="7"/>
       <c r="AQ35" s="7"/>
     </row>
-    <row r="36" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="36" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO36" s="7"/>
       <c r="AP36" s="7"/>
       <c r="AQ36" s="7"/>
     </row>
-    <row r="37" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="37" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO37" s="7"/>
       <c r="AP37" s="7"/>
       <c r="AQ37" s="7"/>
     </row>
-    <row r="38" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="38" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO38" s="7"/>
       <c r="AP38" s="7"/>
       <c r="AQ38" s="7"/>
     </row>
-    <row r="39" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="39" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO39" s="7"/>
       <c r="AP39" s="7"/>
       <c r="AQ39" s="7"/>
     </row>
-    <row r="40" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="40" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO40" s="7"/>
       <c r="AP40" s="7"/>
       <c r="AQ40" s="7"/>
     </row>
-    <row r="41" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="41" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO41" s="7"/>
       <c r="AP41" s="7"/>
       <c r="AQ41" s="7"/>
     </row>
-    <row r="42" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="42" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO42" s="7"/>
       <c r="AP42" s="7"/>
       <c r="AQ42" s="7"/>
     </row>
-    <row r="43" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="43" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO43" s="7"/>
       <c r="AP43" s="7"/>
       <c r="AQ43" s="7"/>
     </row>
-    <row r="44" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="44" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO44" s="7"/>
       <c r="AP44" s="7"/>
       <c r="AQ44" s="7"/>
     </row>
-    <row r="45" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="45" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO45" s="7"/>
       <c r="AP45" s="7"/>
       <c r="AQ45" s="7"/>
     </row>
-    <row r="46" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="46" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO46" s="7"/>
       <c r="AP46" s="7"/>
       <c r="AQ46" s="7"/>
     </row>
-    <row r="47" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="47" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO47" s="7"/>
       <c r="AP47" s="7"/>
       <c r="AQ47" s="7"/>
     </row>
-    <row r="48" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="48" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO48" s="7"/>
       <c r="AP48" s="7"/>
       <c r="AQ48" s="7"/>
     </row>
-    <row r="49" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="49" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO49" s="7"/>
       <c r="AP49" s="7"/>
       <c r="AQ49" s="7"/>
     </row>
-    <row r="50" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="50" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO50" s="7"/>
       <c r="AP50" s="7"/>
       <c r="AQ50" s="7"/>
     </row>
-    <row r="51" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="51" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO51" s="7"/>
       <c r="AP51" s="7"/>
       <c r="AQ51" s="7"/>
     </row>
-    <row r="52" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="52" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO52" s="7"/>
       <c r="AP52" s="7"/>
       <c r="AQ52" s="7"/>
     </row>
-    <row r="53" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="53" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO53" s="7"/>
       <c r="AP53" s="7"/>
       <c r="AQ53" s="7"/>
     </row>
-    <row r="54" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="54" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO54" s="7"/>
       <c r="AP54" s="7"/>
       <c r="AQ54" s="7"/>
     </row>
-    <row r="55" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="55" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO55" s="7"/>
       <c r="AP55" s="7"/>
       <c r="AQ55" s="7"/>
     </row>
-    <row r="56" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="56" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO56" s="7"/>
       <c r="AP56" s="7"/>
       <c r="AQ56" s="7"/>
     </row>
-    <row r="57" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="57" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO57" s="7"/>
       <c r="AP57" s="7"/>
       <c r="AQ57" s="7"/>
     </row>
-    <row r="58" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="58" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO58" s="7"/>
       <c r="AP58" s="7"/>
       <c r="AQ58" s="7"/>
     </row>
-    <row r="59" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="59" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO59" s="7"/>
       <c r="AP59" s="7"/>
       <c r="AQ59" s="7"/>
     </row>
-    <row r="60" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="60" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO60" s="7"/>
       <c r="AP60" s="7"/>
       <c r="AQ60" s="7"/>
     </row>
-    <row r="61" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="61" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO61" s="7"/>
       <c r="AP61" s="7"/>
       <c r="AQ61" s="7"/>
     </row>
-    <row r="62" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="62" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO62" s="7"/>
       <c r="AP62" s="7"/>
       <c r="AQ62" s="7"/>
     </row>
-    <row r="63" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="63" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO63" s="7"/>
       <c r="AP63" s="7"/>
       <c r="AQ63" s="7"/>
     </row>
-    <row r="64" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="64" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO64" s="7"/>
       <c r="AP64" s="7"/>
       <c r="AQ64" s="7"/>
     </row>
-    <row r="65" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="65" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO65" s="7"/>
       <c r="AP65" s="7"/>
       <c r="AQ65" s="7"/>
     </row>
-    <row r="66" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="66" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO66" s="7"/>
       <c r="AP66" s="7"/>
       <c r="AQ66" s="7"/>
     </row>
-    <row r="67" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="67" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO67" s="7"/>
       <c r="AP67" s="7"/>
       <c r="AQ67" s="7"/>
     </row>
-    <row r="68" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="68" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO68" s="7"/>
       <c r="AP68" s="7"/>
       <c r="AQ68" s="7"/>
     </row>
-    <row r="69" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="69" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO69" s="7"/>
       <c r="AP69" s="7"/>
       <c r="AQ69" s="7"/>
     </row>
-    <row r="70" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="70" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO70" s="7"/>
       <c r="AP70" s="7"/>
       <c r="AQ70" s="7"/>
     </row>
-    <row r="71" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="71" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO71" s="7"/>
       <c r="AP71" s="7"/>
       <c r="AQ71" s="7"/>
     </row>
-    <row r="72" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="72" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO72" s="7"/>
       <c r="AP72" s="7"/>
       <c r="AQ72" s="7"/>
     </row>
-    <row r="73" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="73" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO73" s="7"/>
       <c r="AP73" s="7"/>
       <c r="AQ73" s="7"/>
     </row>
-    <row r="74" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="74" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO74" s="7"/>
       <c r="AP74" s="7"/>
       <c r="AQ74" s="7"/>
     </row>
-    <row r="75" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="75" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO75" s="7"/>
       <c r="AP75" s="7"/>
       <c r="AQ75" s="7"/>
     </row>
-    <row r="76" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="76" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO76" s="7"/>
       <c r="AP76" s="7"/>
       <c r="AQ76" s="7"/>
     </row>
-    <row r="77" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="77" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO77" s="7"/>
       <c r="AP77" s="7"/>
       <c r="AQ77" s="7"/>
     </row>
-    <row r="78" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="78" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO78" s="7"/>
       <c r="AP78" s="7"/>
       <c r="AQ78" s="7"/>
     </row>
-    <row r="79" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="79" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO79" s="7"/>
       <c r="AP79" s="7"/>
       <c r="AQ79" s="7"/>
     </row>
-    <row r="80" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="80" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO80" s="7"/>
       <c r="AP80" s="7"/>
       <c r="AQ80" s="7"/>
     </row>
-    <row r="81" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="81" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO81" s="7"/>
       <c r="AP81" s="7"/>
       <c r="AQ81" s="7"/>
     </row>
-    <row r="82" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="82" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO82" s="7"/>
       <c r="AP82" s="7"/>
       <c r="AQ82" s="7"/>
     </row>
-    <row r="83" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="83" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO83" s="7"/>
       <c r="AP83" s="7"/>
       <c r="AQ83" s="7"/>
     </row>
-    <row r="84" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="84" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO84" s="7"/>
       <c r="AP84" s="7"/>
       <c r="AQ84" s="7"/>
     </row>
-    <row r="85" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="85" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO85" s="7"/>
       <c r="AP85" s="7"/>
       <c r="AQ85" s="7"/>
     </row>
-    <row r="86" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="86" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO86" s="7"/>
       <c r="AP86" s="7"/>
       <c r="AQ86" s="7"/>
     </row>
-    <row r="87" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="87" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO87" s="7"/>
       <c r="AP87" s="7"/>
       <c r="AQ87" s="7"/>
     </row>
-    <row r="88" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="88" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO88" s="7"/>
       <c r="AP88" s="7"/>
       <c r="AQ88" s="7"/>
     </row>
-    <row r="89" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="89" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO89" s="7"/>
       <c r="AP89" s="7"/>
       <c r="AQ89" s="7"/>
     </row>
-    <row r="90" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="90" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO90" s="7"/>
       <c r="AP90" s="7"/>
       <c r="AQ90" s="7"/>
     </row>
-    <row r="91" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="91" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO91" s="7"/>
       <c r="AP91" s="7"/>
       <c r="AQ91" s="7"/>
     </row>
-    <row r="92" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="92" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO92" s="7"/>
       <c r="AP92" s="7"/>
       <c r="AQ92" s="7"/>
     </row>
-    <row r="93" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="93" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO93" s="7"/>
       <c r="AP93" s="7"/>
       <c r="AQ93" s="7"/>
     </row>
-    <row r="94" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="94" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO94" s="7"/>
       <c r="AP94" s="7"/>
       <c r="AQ94" s="7"/>
     </row>
-    <row r="95" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="95" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO95" s="7"/>
       <c r="AP95" s="7"/>
       <c r="AQ95" s="7"/>
     </row>
-    <row r="96" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="96" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO96" s="7"/>
       <c r="AP96" s="7"/>
       <c r="AQ96" s="7"/>
     </row>
-    <row r="97" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="97" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO97" s="7"/>
       <c r="AP97" s="7"/>
       <c r="AQ97" s="7"/>
     </row>
-    <row r="98" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="98" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO98" s="7"/>
       <c r="AP98" s="7"/>
       <c r="AQ98" s="7"/>
     </row>
-    <row r="99" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="99" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO99" s="7"/>
       <c r="AP99" s="7"/>
       <c r="AQ99" s="7"/>
     </row>
-    <row r="100" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="100" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO100" s="7"/>
       <c r="AP100" s="7"/>
       <c r="AQ100" s="7"/>
     </row>
-    <row r="101" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="101" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO101" s="7"/>
       <c r="AP101" s="7"/>
       <c r="AQ101" s="7"/>
     </row>
-    <row r="102" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="102" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO102" s="7"/>
       <c r="AP102" s="7"/>
       <c r="AQ102" s="7"/>
     </row>
-    <row r="103" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="103" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO103" s="7"/>
       <c r="AP103" s="7"/>
       <c r="AQ103" s="7"/>
     </row>
-    <row r="104" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="104" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO104" s="7"/>
       <c r="AP104" s="7"/>
       <c r="AQ104" s="7"/>
     </row>
-    <row r="105" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="105" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO105" s="7"/>
       <c r="AP105" s="7"/>
       <c r="AQ105" s="7"/>
     </row>
-    <row r="106" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="106" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO106" s="7"/>
       <c r="AP106" s="7"/>
       <c r="AQ106" s="7"/>
     </row>
-    <row r="107" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="107" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO107" s="7"/>
       <c r="AP107" s="7"/>
       <c r="AQ107" s="7"/>
     </row>
-    <row r="108" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="108" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO108" s="7"/>
       <c r="AP108" s="7"/>
       <c r="AQ108" s="7"/>
     </row>
-    <row r="109" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="109" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO109" s="7"/>
       <c r="AP109" s="7"/>
       <c r="AQ109" s="7"/>
     </row>
-    <row r="110" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="110" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO110" s="7"/>
       <c r="AP110" s="7"/>
       <c r="AQ110" s="7"/>
     </row>
-    <row r="111" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="111" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO111" s="7"/>
       <c r="AP111" s="7"/>
       <c r="AQ111" s="7"/>
     </row>
-    <row r="112" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="112" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO112" s="7"/>
       <c r="AP112" s="7"/>
       <c r="AQ112" s="7"/>
     </row>
-    <row r="113" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="113" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO113" s="7"/>
       <c r="AP113" s="7"/>
       <c r="AQ113" s="7"/>
     </row>
-    <row r="114" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="114" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO114" s="7"/>
       <c r="AP114" s="7"/>
       <c r="AQ114" s="7"/>
     </row>
-    <row r="115" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="115" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO115" s="7"/>
       <c r="AP115" s="7"/>
       <c r="AQ115" s="7"/>
     </row>
-    <row r="116" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="116" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO116" s="7"/>
       <c r="AP116" s="7"/>
       <c r="AQ116" s="7"/>
     </row>
-    <row r="117" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="117" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO117" s="7"/>
       <c r="AP117" s="7"/>
       <c r="AQ117" s="7"/>
     </row>
-    <row r="118" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="118" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO118" s="7"/>
       <c r="AP118" s="7"/>
       <c r="AQ118" s="7"/>
     </row>
-    <row r="119" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="119" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO119" s="7"/>
       <c r="AP119" s="7"/>
       <c r="AQ119" s="7"/>
     </row>
-    <row r="120" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="120" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO120" s="7"/>
       <c r="AP120" s="7"/>
       <c r="AQ120" s="7"/>
     </row>
-    <row r="121" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="121" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO121" s="7"/>
       <c r="AP121" s="7"/>
       <c r="AQ121" s="7"/>
     </row>
-    <row r="122" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="122" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO122" s="7"/>
       <c r="AP122" s="7"/>
       <c r="AQ122" s="7"/>
     </row>
-    <row r="123" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="123" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO123" s="7"/>
       <c r="AP123" s="7"/>
       <c r="AQ123" s="7"/>
     </row>
-    <row r="124" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="124" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO124" s="7"/>
       <c r="AP124" s="7"/>
       <c r="AQ124" s="7"/>
     </row>
-    <row r="125" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="125" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO125" s="7"/>
       <c r="AP125" s="7"/>
       <c r="AQ125" s="7"/>
     </row>
-    <row r="126" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="126" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO126" s="7"/>
       <c r="AP126" s="7"/>
       <c r="AQ126" s="7"/>
     </row>
-    <row r="127" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="127" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO127" s="7"/>
       <c r="AP127" s="7"/>
       <c r="AQ127" s="7"/>
     </row>
-    <row r="128" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="128" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO128" s="7"/>
       <c r="AP128" s="7"/>
       <c r="AQ128" s="7"/>
     </row>
-    <row r="129" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="129" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO129" s="7"/>
       <c r="AP129" s="7"/>
       <c r="AQ129" s="7"/>
     </row>
-    <row r="130" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="130" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO130" s="7"/>
       <c r="AP130" s="7"/>
       <c r="AQ130" s="7"/>
     </row>
-    <row r="131" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="131" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO131" s="7"/>
       <c r="AP131" s="7"/>
       <c r="AQ131" s="7"/>
     </row>
-    <row r="132" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="132" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO132" s="7"/>
       <c r="AP132" s="7"/>
       <c r="AQ132" s="7"/>
     </row>
-    <row r="133" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="133" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO133" s="7"/>
       <c r="AP133" s="7"/>
       <c r="AQ133" s="7"/>
     </row>
-    <row r="134" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="134" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO134" s="7"/>
       <c r="AP134" s="7"/>
       <c r="AQ134" s="7"/>
     </row>
-    <row r="135" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="135" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO135" s="7"/>
       <c r="AP135" s="7"/>
       <c r="AQ135" s="7"/>
     </row>
-    <row r="136" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="136" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO136" s="7"/>
       <c r="AP136" s="7"/>
       <c r="AQ136" s="7"/>
     </row>
-    <row r="137" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="137" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO137" s="7"/>
       <c r="AP137" s="7"/>
       <c r="AQ137" s="7"/>
     </row>
-    <row r="138" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="138" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO138" s="7"/>
       <c r="AP138" s="7"/>
       <c r="AQ138" s="7"/>
     </row>
-    <row r="139" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="139" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO139" s="7"/>
       <c r="AP139" s="7"/>
       <c r="AQ139" s="7"/>
     </row>
-    <row r="140" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="140" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO140" s="7"/>
       <c r="AP140" s="7"/>
       <c r="AQ140" s="7"/>
     </row>
-    <row r="141" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="141" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO141" s="7"/>
       <c r="AP141" s="7"/>
       <c r="AQ141" s="7"/>
     </row>
-    <row r="142" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="142" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO142" s="7"/>
       <c r="AP142" s="7"/>
       <c r="AQ142" s="7"/>
     </row>
-    <row r="143" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="143" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO143" s="7"/>
       <c r="AP143" s="7"/>
       <c r="AQ143" s="7"/>
     </row>
-    <row r="144" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="144" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO144" s="7"/>
       <c r="AP144" s="7"/>
       <c r="AQ144" s="7"/>
     </row>
-    <row r="145" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="145" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO145" s="7"/>
       <c r="AP145" s="7"/>
       <c r="AQ145" s="7"/>
     </row>
-    <row r="146" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="146" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO146" s="7"/>
       <c r="AP146" s="7"/>
       <c r="AQ146" s="7"/>
     </row>
-    <row r="147" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="147" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO147" s="7"/>
       <c r="AP147" s="7"/>
       <c r="AQ147" s="7"/>
     </row>
-    <row r="148" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="148" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO148" s="7"/>
       <c r="AP148" s="7"/>
       <c r="AQ148" s="7"/>
     </row>
-    <row r="149" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="149" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO149" s="7"/>
       <c r="AP149" s="7"/>
       <c r="AQ149" s="7"/>
     </row>
-    <row r="150" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="150" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO150" s="7"/>
       <c r="AP150" s="7"/>
       <c r="AQ150" s="7"/>
     </row>
-    <row r="151" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="151" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO151" s="7"/>
       <c r="AP151" s="7"/>
       <c r="AQ151" s="7"/>
     </row>
-    <row r="152" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="152" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO152" s="7"/>
       <c r="AP152" s="7"/>
       <c r="AQ152" s="7"/>
     </row>
-    <row r="153" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="153" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO153" s="7"/>
       <c r="AP153" s="7"/>
       <c r="AQ153" s="7"/>
     </row>
-    <row r="154" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="154" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO154" s="7"/>
       <c r="AP154" s="7"/>
       <c r="AQ154" s="7"/>
     </row>
-    <row r="155" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="155" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO155" s="7"/>
       <c r="AP155" s="7"/>
       <c r="AQ155" s="7"/>
     </row>
-    <row r="156" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="156" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO156" s="7"/>
       <c r="AP156" s="7"/>
       <c r="AQ156" s="7"/>
     </row>
-    <row r="157" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="157" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO157" s="7"/>
       <c r="AP157" s="7"/>
       <c r="AQ157" s="7"/>
     </row>
-    <row r="158" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="158" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO158" s="7"/>
       <c r="AP158" s="7"/>
       <c r="AQ158" s="7"/>
     </row>
-    <row r="159" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="159" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO159" s="7"/>
       <c r="AP159" s="7"/>
       <c r="AQ159" s="7"/>
     </row>
-    <row r="160" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="160" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO160" s="7"/>
       <c r="AP160" s="7"/>
       <c r="AQ160" s="7"/>
     </row>
-    <row r="161" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="161" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO161" s="7"/>
       <c r="AP161" s="7"/>
       <c r="AQ161" s="7"/>
     </row>
-    <row r="162" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="162" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO162" s="7"/>
       <c r="AP162" s="7"/>
       <c r="AQ162" s="7"/>
     </row>
-    <row r="163" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="163" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO163" s="7"/>
       <c r="AP163" s="7"/>
       <c r="AQ163" s="7"/>
     </row>
-    <row r="164" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="164" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO164" s="7"/>
       <c r="AP164" s="7"/>
       <c r="AQ164" s="7"/>
     </row>
-    <row r="165" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="165" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO165" s="7"/>
       <c r="AP165" s="7"/>
       <c r="AQ165" s="7"/>
     </row>
-    <row r="166" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="166" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO166" s="7"/>
       <c r="AP166" s="7"/>
       <c r="AQ166" s="7"/>
     </row>
-    <row r="167" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="167" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO167" s="7"/>
       <c r="AP167" s="7"/>
       <c r="AQ167" s="7"/>
     </row>
-    <row r="168" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="168" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO168" s="7"/>
       <c r="AP168" s="7"/>
       <c r="AQ168" s="7"/>
     </row>
-    <row r="169" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="169" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO169" s="7"/>
       <c r="AP169" s="7"/>
       <c r="AQ169" s="7"/>
     </row>
-    <row r="170" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="170" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO170" s="7"/>
       <c r="AP170" s="7"/>
       <c r="AQ170" s="7"/>
     </row>
-    <row r="171" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="171" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO171" s="7"/>
       <c r="AP171" s="7"/>
       <c r="AQ171" s="7"/>
     </row>
-    <row r="172" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="172" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO172" s="7"/>
       <c r="AP172" s="7"/>
       <c r="AQ172" s="7"/>
     </row>
-    <row r="173" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="173" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO173" s="7"/>
       <c r="AP173" s="7"/>
       <c r="AQ173" s="7"/>
     </row>
-    <row r="174" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="174" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO174" s="7"/>
       <c r="AP174" s="7"/>
       <c r="AQ174" s="7"/>
     </row>
-    <row r="175" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="175" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO175" s="7"/>
       <c r="AP175" s="7"/>
       <c r="AQ175" s="7"/>
     </row>
-    <row r="176" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="176" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO176" s="7"/>
       <c r="AP176" s="7"/>
       <c r="AQ176" s="7"/>
     </row>
-    <row r="177" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="177" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO177" s="7"/>
       <c r="AP177" s="7"/>
       <c r="AQ177" s="7"/>
     </row>
-    <row r="178" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="178" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO178" s="7"/>
       <c r="AP178" s="7"/>
       <c r="AQ178" s="7"/>
     </row>
-    <row r="179" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="179" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO179" s="7"/>
       <c r="AP179" s="7"/>
       <c r="AQ179" s="7"/>
     </row>
-    <row r="180" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="180" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO180" s="7"/>
       <c r="AP180" s="7"/>
       <c r="AQ180" s="7"/>
     </row>
-    <row r="181" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="181" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO181" s="7"/>
       <c r="AP181" s="7"/>
       <c r="AQ181" s="7"/>
     </row>
-    <row r="182" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="182" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO182" s="7"/>
       <c r="AP182" s="7"/>
       <c r="AQ182" s="7"/>
     </row>
-    <row r="183" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="183" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO183" s="7"/>
       <c r="AP183" s="7"/>
       <c r="AQ183" s="7"/>
     </row>
-    <row r="184" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="184" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO184" s="7"/>
       <c r="AP184" s="7"/>
       <c r="AQ184" s="7"/>
     </row>
-    <row r="185" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="185" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO185" s="7"/>
       <c r="AP185" s="7"/>
       <c r="AQ185" s="7"/>
     </row>
-    <row r="186" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="186" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO186" s="7"/>
       <c r="AP186" s="7"/>
       <c r="AQ186" s="7"/>
     </row>
-    <row r="187" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="187" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO187" s="7"/>
       <c r="AP187" s="7"/>
       <c r="AQ187" s="7"/>
     </row>
-    <row r="188" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="188" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO188" s="7"/>
       <c r="AP188" s="7"/>
       <c r="AQ188" s="7"/>
     </row>
-    <row r="189" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="189" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO189" s="7"/>
       <c r="AP189" s="7"/>
       <c r="AQ189" s="7"/>
     </row>
-    <row r="190" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="190" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO190" s="7"/>
       <c r="AP190" s="7"/>
       <c r="AQ190" s="7"/>
     </row>
-    <row r="191" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="191" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO191" s="7"/>
       <c r="AP191" s="7"/>
       <c r="AQ191" s="7"/>
     </row>
-    <row r="192" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="192" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO192" s="7"/>
       <c r="AP192" s="7"/>
       <c r="AQ192" s="7"/>
     </row>
-    <row r="193" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="193" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO193" s="7"/>
       <c r="AP193" s="7"/>
       <c r="AQ193" s="7"/>
     </row>
-    <row r="194" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="194" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO194" s="7"/>
       <c r="AP194" s="7"/>
       <c r="AQ194" s="7"/>
     </row>
-    <row r="195" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="195" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO195" s="7"/>
       <c r="AP195" s="7"/>
       <c r="AQ195" s="7"/>
     </row>
-    <row r="196" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="196" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO196" s="7"/>
       <c r="AP196" s="7"/>
       <c r="AQ196" s="7"/>
     </row>
-    <row r="197" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="197" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO197" s="7"/>
       <c r="AP197" s="7"/>
       <c r="AQ197" s="7"/>
     </row>
-    <row r="198" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="198" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO198" s="7"/>
       <c r="AP198" s="7"/>
       <c r="AQ198" s="7"/>
     </row>
-    <row r="199" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="199" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO199" s="7"/>
       <c r="AP199" s="7"/>
       <c r="AQ199" s="7"/>
     </row>
-    <row r="200" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="200" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO200" s="7"/>
       <c r="AP200" s="7"/>
       <c r="AQ200" s="7"/>
     </row>
-    <row r="201" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="201" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO201" s="7"/>
       <c r="AP201" s="7"/>
       <c r="AQ201" s="7"/>
     </row>
-    <row r="202" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="202" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO202" s="7"/>
       <c r="AP202" s="7"/>
       <c r="AQ202" s="7"/>
     </row>
-    <row r="203" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="203" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO203" s="7"/>
       <c r="AP203" s="7"/>
       <c r="AQ203" s="7"/>
     </row>
-    <row r="204" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="204" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO204" s="7"/>
       <c r="AP204" s="7"/>
       <c r="AQ204" s="7"/>
     </row>
-    <row r="205" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="205" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO205" s="7"/>
       <c r="AP205" s="7"/>
       <c r="AQ205" s="7"/>
     </row>
-    <row r="206" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="206" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO206" s="7"/>
       <c r="AP206" s="7"/>
       <c r="AQ206" s="7"/>
     </row>
-    <row r="207" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="207" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO207" s="7"/>
       <c r="AP207" s="7"/>
       <c r="AQ207" s="7"/>
     </row>
-    <row r="208" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="208" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO208" s="7"/>
       <c r="AP208" s="7"/>
       <c r="AQ208" s="7"/>
     </row>
-    <row r="209" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="209" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO209" s="7"/>
       <c r="AP209" s="7"/>
       <c r="AQ209" s="7"/>
     </row>
-    <row r="210" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="210" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO210" s="7"/>
       <c r="AP210" s="7"/>
       <c r="AQ210" s="7"/>
     </row>
-    <row r="211" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="211" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO211" s="7"/>
       <c r="AP211" s="7"/>
       <c r="AQ211" s="7"/>
     </row>
-    <row r="212" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="212" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO212" s="7"/>
       <c r="AP212" s="7"/>
       <c r="AQ212" s="7"/>
     </row>
-    <row r="213" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="213" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO213" s="7"/>
       <c r="AP213" s="7"/>
       <c r="AQ213" s="7"/>
     </row>
-    <row r="214" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="214" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO214" s="7"/>
       <c r="AP214" s="7"/>
       <c r="AQ214" s="7"/>
     </row>
-    <row r="215" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="215" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO215" s="7"/>
       <c r="AP215" s="7"/>
       <c r="AQ215" s="7"/>
     </row>
-    <row r="216" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="216" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO216" s="7"/>
       <c r="AP216" s="7"/>
       <c r="AQ216" s="7"/>
     </row>
-    <row r="217" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="217" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO217" s="7"/>
       <c r="AP217" s="7"/>
       <c r="AQ217" s="7"/>
     </row>
-    <row r="218" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="218" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO218" s="7"/>
       <c r="AP218" s="7"/>
       <c r="AQ218" s="7"/>
     </row>
-    <row r="219" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="219" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO219" s="7"/>
       <c r="AP219" s="7"/>
       <c r="AQ219" s="7"/>
     </row>
-    <row r="220" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="220" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO220" s="7"/>
       <c r="AP220" s="7"/>
       <c r="AQ220" s="7"/>
     </row>
-    <row r="221" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="221" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO221" s="7"/>
       <c r="AP221" s="7"/>
       <c r="AQ221" s="7"/>
     </row>
-    <row r="222" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="222" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO222" s="7"/>
       <c r="AP222" s="7"/>
       <c r="AQ222" s="7"/>
     </row>
-    <row r="223" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="223" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO223" s="7"/>
       <c r="AP223" s="7"/>
       <c r="AQ223" s="7"/>
     </row>
-    <row r="224" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="224" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO224" s="7"/>
       <c r="AP224" s="7"/>
       <c r="AQ224" s="7"/>
     </row>
-    <row r="225" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="225" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO225" s="7"/>
       <c r="AP225" s="7"/>
       <c r="AQ225" s="7"/>
     </row>
-    <row r="226" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="226" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO226" s="7"/>
       <c r="AP226" s="7"/>
       <c r="AQ226" s="7"/>
     </row>
-    <row r="227" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="227" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO227" s="7"/>
       <c r="AP227" s="7"/>
       <c r="AQ227" s="7"/>
     </row>
-    <row r="228" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="228" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO228" s="7"/>
       <c r="AP228" s="7"/>
       <c r="AQ228" s="7"/>
     </row>
-    <row r="229" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="229" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO229" s="7"/>
       <c r="AP229" s="7"/>
       <c r="AQ229" s="7"/>
     </row>
-    <row r="230" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="230" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO230" s="7"/>
       <c r="AP230" s="7"/>
       <c r="AQ230" s="7"/>
     </row>
-    <row r="231" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="231" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO231" s="7"/>
       <c r="AP231" s="7"/>
       <c r="AQ231" s="7"/>
     </row>
-    <row r="232" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="232" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO232" s="7"/>
       <c r="AP232" s="7"/>
       <c r="AQ232" s="7"/>
     </row>
-    <row r="233" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="233" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO233" s="7"/>
       <c r="AP233" s="7"/>
       <c r="AQ233" s="7"/>
     </row>
-    <row r="234" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="234" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO234" s="7"/>
       <c r="AP234" s="7"/>
       <c r="AQ234" s="7"/>
     </row>
-    <row r="235" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="235" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO235" s="7"/>
       <c r="AP235" s="7"/>
       <c r="AQ235" s="7"/>
     </row>
-    <row r="236" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="236" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO236" s="7"/>
       <c r="AP236" s="7"/>
       <c r="AQ236" s="7"/>
     </row>
-    <row r="237" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="237" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO237" s="7"/>
       <c r="AP237" s="7"/>
       <c r="AQ237" s="7"/>
     </row>
-    <row r="238" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="238" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO238" s="7"/>
       <c r="AP238" s="7"/>
       <c r="AQ238" s="7"/>
     </row>
-    <row r="239" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="239" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO239" s="7"/>
       <c r="AP239" s="7"/>
       <c r="AQ239" s="7"/>
     </row>
-    <row r="240" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="240" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO240" s="7"/>
       <c r="AP240" s="7"/>
       <c r="AQ240" s="7"/>
     </row>
-    <row r="241" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="241" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO241" s="7"/>
       <c r="AP241" s="7"/>
       <c r="AQ241" s="7"/>
     </row>
-    <row r="242" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="242" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO242" s="7"/>
       <c r="AP242" s="7"/>
       <c r="AQ242" s="7"/>
     </row>
-    <row r="243" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="243" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO243" s="7"/>
       <c r="AP243" s="7"/>
       <c r="AQ243" s="7"/>
     </row>
-    <row r="244" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="244" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO244" s="7"/>
       <c r="AP244" s="7"/>
       <c r="AQ244" s="7"/>
     </row>
-    <row r="245" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="245" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO245" s="7"/>
       <c r="AP245" s="7"/>
       <c r="AQ245" s="7"/>
     </row>
-    <row r="246" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="246" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO246" s="7"/>
       <c r="AP246" s="7"/>
       <c r="AQ246" s="7"/>
     </row>
-    <row r="247" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="247" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO247" s="7"/>
       <c r="AP247" s="7"/>
       <c r="AQ247" s="7"/>
     </row>
-    <row r="248" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="248" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO248" s="7"/>
       <c r="AP248" s="7"/>
       <c r="AQ248" s="7"/>
     </row>
-    <row r="249" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="249" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO249" s="7"/>
       <c r="AP249" s="7"/>
       <c r="AQ249" s="7"/>
     </row>
-    <row r="250" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="250" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO250" s="7"/>
       <c r="AP250" s="7"/>
       <c r="AQ250" s="7"/>
     </row>
-    <row r="251" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="251" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO251" s="7"/>
       <c r="AP251" s="7"/>
       <c r="AQ251" s="7"/>
     </row>
-    <row r="252" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="252" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO252" s="7"/>
       <c r="AP252" s="7"/>
       <c r="AQ252" s="7"/>
     </row>
-    <row r="253" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="253" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO253" s="7"/>
       <c r="AP253" s="7"/>
       <c r="AQ253" s="7"/>
     </row>
-    <row r="254" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="254" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO254" s="7"/>
       <c r="AP254" s="7"/>
       <c r="AQ254" s="7"/>
     </row>
-    <row r="255" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="255" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO255" s="7"/>
       <c r="AP255" s="7"/>
       <c r="AQ255" s="7"/>
     </row>
-    <row r="256" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="256" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO256" s="7"/>
       <c r="AP256" s="7"/>
       <c r="AQ256" s="7"/>
     </row>
-    <row r="257" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="257" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO257" s="7"/>
       <c r="AP257" s="7"/>
       <c r="AQ257" s="7"/>
     </row>
-    <row r="258" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="258" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO258" s="7"/>
       <c r="AP258" s="7"/>
       <c r="AQ258" s="7"/>
     </row>
-    <row r="259" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="259" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO259" s="7"/>
       <c r="AP259" s="7"/>
       <c r="AQ259" s="7"/>
     </row>
-    <row r="260" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="260" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO260" s="7"/>
       <c r="AP260" s="7"/>
       <c r="AQ260" s="7"/>
     </row>
-    <row r="261" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="261" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO261" s="7"/>
       <c r="AP261" s="7"/>
       <c r="AQ261" s="7"/>
     </row>
-    <row r="262" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="262" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO262" s="7"/>
       <c r="AP262" s="7"/>
       <c r="AQ262" s="7"/>
     </row>
-    <row r="263" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="263" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO263" s="7"/>
       <c r="AP263" s="7"/>
       <c r="AQ263" s="7"/>
     </row>
-    <row r="264" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="264" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO264" s="7"/>
       <c r="AP264" s="7"/>
       <c r="AQ264" s="7"/>
     </row>
-    <row r="265" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="265" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO265" s="7"/>
       <c r="AP265" s="7"/>
       <c r="AQ265" s="7"/>
     </row>
-    <row r="266" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="266" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO266" s="7"/>
       <c r="AP266" s="7"/>
       <c r="AQ266" s="7"/>
     </row>
-    <row r="267" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="267" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO267" s="7"/>
       <c r="AP267" s="7"/>
       <c r="AQ267" s="7"/>
     </row>
-    <row r="268" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="268" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO268" s="7"/>
       <c r="AP268" s="7"/>
       <c r="AQ268" s="7"/>
     </row>
-    <row r="269" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="269" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO269" s="7"/>
       <c r="AP269" s="7"/>
       <c r="AQ269" s="7"/>
     </row>
-    <row r="270" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="270" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO270" s="7"/>
       <c r="AP270" s="7"/>
       <c r="AQ270" s="7"/>
     </row>
-    <row r="271" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="271" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO271" s="7"/>
       <c r="AP271" s="7"/>
       <c r="AQ271" s="7"/>
     </row>
-    <row r="272" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="272" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO272" s="7"/>
       <c r="AP272" s="7"/>
       <c r="AQ272" s="7"/>
     </row>
-    <row r="273" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="273" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO273" s="7"/>
       <c r="AP273" s="7"/>
       <c r="AQ273" s="7"/>
     </row>
-    <row r="274" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="274" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO274" s="7"/>
       <c r="AP274" s="7"/>
       <c r="AQ274" s="7"/>
     </row>
-    <row r="275" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="275" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO275" s="7"/>
       <c r="AP275" s="7"/>
       <c r="AQ275" s="7"/>
     </row>
-    <row r="276" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="276" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO276" s="7"/>
       <c r="AP276" s="7"/>
       <c r="AQ276" s="7"/>
     </row>
-    <row r="277" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="277" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO277" s="7"/>
       <c r="AP277" s="7"/>
       <c r="AQ277" s="7"/>
     </row>
-    <row r="278" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="278" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO278" s="7"/>
       <c r="AP278" s="7"/>
       <c r="AQ278" s="7"/>
     </row>
-    <row r="279" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="279" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO279" s="7"/>
       <c r="AP279" s="7"/>
       <c r="AQ279" s="7"/>
     </row>
-    <row r="280" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="280" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO280" s="7"/>
       <c r="AP280" s="7"/>
       <c r="AQ280" s="7"/>
     </row>
-    <row r="281" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="281" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO281" s="7"/>
       <c r="AP281" s="7"/>
       <c r="AQ281" s="7"/>
     </row>
-    <row r="282" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="282" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO282" s="7"/>
       <c r="AP282" s="7"/>
       <c r="AQ282" s="7"/>
     </row>
-    <row r="283" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="283" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO283" s="7"/>
       <c r="AP283" s="7"/>
       <c r="AQ283" s="7"/>
     </row>
-    <row r="284" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="284" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO284" s="7"/>
       <c r="AP284" s="7"/>
       <c r="AQ284" s="7"/>
     </row>
-    <row r="285" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="285" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO285" s="7"/>
       <c r="AP285" s="7"/>
       <c r="AQ285" s="7"/>
     </row>
-    <row r="286" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="286" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO286" s="7"/>
       <c r="AP286" s="7"/>
       <c r="AQ286" s="7"/>
     </row>
-    <row r="287" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="287" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO287" s="7"/>
       <c r="AP287" s="7"/>
       <c r="AQ287" s="7"/>
     </row>
-    <row r="288" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="288" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO288" s="7"/>
       <c r="AP288" s="7"/>
       <c r="AQ288" s="7"/>
     </row>
-    <row r="289" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="289" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO289" s="7"/>
       <c r="AP289" s="7"/>
       <c r="AQ289" s="7"/>
     </row>
-    <row r="290" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="290" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO290" s="7"/>
       <c r="AP290" s="7"/>
       <c r="AQ290" s="7"/>
     </row>
-    <row r="291" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="291" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO291" s="7"/>
       <c r="AP291" s="7"/>
       <c r="AQ291" s="7"/>
     </row>
-    <row r="292" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="292" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO292" s="7"/>
       <c r="AP292" s="7"/>
       <c r="AQ292" s="7"/>
     </row>
-    <row r="293" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="293" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO293" s="7"/>
       <c r="AP293" s="7"/>
       <c r="AQ293" s="7"/>
     </row>
-    <row r="294" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="294" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO294" s="7"/>
       <c r="AP294" s="7"/>
       <c r="AQ294" s="7"/>
     </row>
-    <row r="295" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="295" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO295" s="7"/>
       <c r="AP295" s="7"/>
       <c r="AQ295" s="7"/>
     </row>
-    <row r="296" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="296" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO296" s="7"/>
       <c r="AP296" s="7"/>
       <c r="AQ296" s="7"/>
     </row>
-    <row r="297" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="297" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO297" s="7"/>
       <c r="AP297" s="7"/>
       <c r="AQ297" s="7"/>
     </row>
-    <row r="298" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="298" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO298" s="7"/>
       <c r="AP298" s="7"/>
       <c r="AQ298" s="7"/>
     </row>
-    <row r="299" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="299" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO299" s="7"/>
       <c r="AP299" s="7"/>
       <c r="AQ299" s="7"/>
     </row>
-    <row r="300" spans="41:43" x14ac:dyDescent="0.2">
+    <row r="300" spans="41:43" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AO300" s="7"/>
       <c r="AP300" s="7"/>
       <c r="AQ300" s="7"/>

</xml_diff>